<commit_message>
Update inventário_fuji - 12-05.xlsx
</commit_message>
<xml_diff>
--- a/inventário_fuji - 12-05.xlsx
+++ b/inventário_fuji - 12-05.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cauac\OneDrive\Área de Trabalho\FUJI\Gerenciamento de Estoque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cauac\OneDrive\Área de Trabalho\FUJI\Gerenciamento de Estoque\FujiStock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C443BC1-A18D-4143-95D9-F1173E901280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F33B39E-F2C5-45CE-88FE-7B07B5840007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="3" xr2:uid="{CC8599C9-BADD-4EB1-B3D7-3F9205998A6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC8599C9-BADD-4EB1-B3D7-3F9205998A6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Bebidas Estoque Seco" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="167">
   <si>
     <t>Categoria</t>
   </si>
@@ -530,9 +530,6 @@
   </si>
   <si>
     <t>Licores e Aperitivos</t>
-  </si>
-  <si>
-    <t>Vinhos</t>
   </si>
   <si>
     <t>Pães e Massas</t>
@@ -1212,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C854C540-1A53-4E3B-AFAD-692006BCF0EE}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1244,7 @@
         <v>45789</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>6</v>
@@ -1264,7 +1261,7 @@
         <v>45789</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>7</v>
@@ -1281,7 +1278,7 @@
         <v>45789</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>8</v>
@@ -1298,7 +1295,7 @@
         <v>45789</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>9</v>
@@ -1587,7 +1584,7 @@
         <v>45789</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>28</v>
@@ -1604,7 +1601,7 @@
         <v>45789</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>29</v>
@@ -1621,7 +1618,7 @@
         <v>45789</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>30</v>
@@ -1638,7 +1635,7 @@
         <v>45789</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>31</v>
@@ -1655,7 +1652,7 @@
         <v>45789</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>32</v>
@@ -1672,7 +1669,7 @@
         <v>45789</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>33</v>
@@ -1689,7 +1686,7 @@
         <v>45789</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>34</v>
@@ -1706,7 +1703,7 @@
         <v>45789</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>35</v>
@@ -1723,7 +1720,7 @@
         <v>45789</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>36</v>
@@ -1740,7 +1737,7 @@
         <v>45789</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>37</v>
@@ -1774,7 +1771,7 @@
         <v>45789</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>39</v>
@@ -1791,7 +1788,7 @@
         <v>45789</v>
       </c>
       <c r="B34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="28" t="s">
         <v>40</v>
@@ -1808,7 +1805,7 @@
         <v>45789</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>41</v>
@@ -1825,7 +1822,7 @@
         <v>45789</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>42</v>
@@ -1842,7 +1839,7 @@
         <v>45789</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C37" s="28" t="s">
         <v>43</v>
@@ -1859,7 +1856,7 @@
         <v>45789</v>
       </c>
       <c r="B38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>44</v>
@@ -1876,7 +1873,7 @@
         <v>45789</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C39" s="28" t="s">
         <v>45</v>
@@ -1893,7 +1890,7 @@
         <v>45789</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>46</v>
@@ -1910,7 +1907,7 @@
         <v>45789</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="28" t="s">
         <v>47</v>
@@ -2114,7 +2111,7 @@
         <v>45789</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" s="28" t="s">
         <v>53</v>
@@ -2131,7 +2128,7 @@
         <v>45789</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C54" s="28" t="s">
         <v>54</v>
@@ -2188,7 +2185,7 @@
         <v>45789</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>61</v>
@@ -2205,7 +2202,7 @@
         <v>45789</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>62</v>
@@ -2222,7 +2219,7 @@
         <v>45789</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>63</v>
@@ -2239,7 +2236,7 @@
         <v>45789</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>64</v>
@@ -2256,7 +2253,7 @@
         <v>45789</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>65</v>
@@ -2273,7 +2270,7 @@
         <v>45789</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>66</v>
@@ -2290,7 +2287,7 @@
         <v>45789</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>67</v>
@@ -2307,7 +2304,7 @@
         <v>45789</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>68</v>
@@ -2324,7 +2321,7 @@
         <v>45789</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>69</v>
@@ -2341,7 +2338,7 @@
         <v>45789</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>70</v>
@@ -2358,7 +2355,7 @@
         <v>45789</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>71</v>
@@ -2375,7 +2372,7 @@
         <v>45789</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>72</v>
@@ -2392,7 +2389,7 @@
         <v>45789</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>73</v>
@@ -2600,7 +2597,7 @@
         <v>45789</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>76</v>
@@ -2617,7 +2614,7 @@
         <v>45789</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>77</v>
@@ -2634,7 +2631,7 @@
         <v>45789</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>78</v>
@@ -2651,7 +2648,7 @@
         <v>45789</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>79</v>
@@ -2668,7 +2665,7 @@
         <v>45789</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>80</v>
@@ -2685,7 +2682,7 @@
         <v>45789</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>81</v>
@@ -2702,7 +2699,7 @@
         <v>45789</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>82</v>
@@ -2719,7 +2716,7 @@
         <v>45789</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>83</v>
@@ -2736,7 +2733,7 @@
         <v>45789</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>84</v>
@@ -2753,7 +2750,7 @@
         <v>45789</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>85</v>
@@ -2770,7 +2767,7 @@
         <v>45789</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>86</v>
@@ -2787,7 +2784,7 @@
         <v>45789</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>87</v>
@@ -2809,7 +2806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0ADCD2A-F426-41F5-A5D4-BD2EA62EB2B1}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2844,7 +2841,7 @@
         <v>45789</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>105</v>
@@ -2963,7 +2960,7 @@
         <v>45789</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>111</v>
@@ -2980,7 +2977,7 @@
         <v>45789</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>104</v>
@@ -2998,7 +2995,7 @@
         <v>45789</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>103</v>
@@ -3015,7 +3012,7 @@
         <v>45789</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>102</v>
@@ -3049,7 +3046,7 @@
         <v>45789</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>95</v>
@@ -3066,7 +3063,7 @@
         <v>45789</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>96</v>
@@ -3083,7 +3080,7 @@
         <v>45789</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>97</v>
@@ -3100,7 +3097,7 @@
         <v>45789</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>98</v>
@@ -3117,7 +3114,7 @@
         <v>45789</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>99</v>
@@ -3134,7 +3131,7 @@
         <v>45789</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>100</v>
@@ -3276,7 +3273,7 @@
         <v>45789</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>151</v>
@@ -3293,7 +3290,7 @@
         <v>45789</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>152</v>
@@ -3310,7 +3307,7 @@
         <v>45789</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>153</v>
@@ -3327,7 +3324,7 @@
         <v>45789</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>78</v>
@@ -3344,7 +3341,7 @@
         <v>45789</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>154</v>
@@ -3361,7 +3358,7 @@
         <v>45789</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>155</v>
@@ -3378,7 +3375,7 @@
         <v>45789</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>156</v>
@@ -3395,7 +3392,7 @@
         <v>45789</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>157</v>
@@ -3412,7 +3409,7 @@
         <v>45789</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>158</v>
@@ -3533,7 +3530,7 @@
         <v>45789</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>116</v>
@@ -4085,7 +4082,7 @@
         <v>45789</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>146</v>
@@ -4119,7 +4116,7 @@
         <v>45789</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>148</v>
@@ -4136,7 +4133,7 @@
         <v>45789</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>149</v>

</xml_diff>